<commit_message>
implemented parameter bounds and observation weights
</commit_message>
<xml_diff>
--- a/data/weights.xlsx
+++ b/data/weights.xlsx
@@ -1,64 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C91A66-E9DF-F749-BC1B-A5C43AEBAAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23840" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sigma</t>
   </si>
   <si>
-    <t>unity</t>
-  </si>
-  <si>
-    <t>head</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>m3/h</t>
-  </si>
-  <si>
-    <t>discharge</t>
-  </si>
-  <si>
-    <t>mixing_ratio</t>
-  </si>
-  <si>
     <t>data_types</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>tuning_factor</t>
-  </si>
-  <si>
-    <t>fluc_head</t>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>heads</t>
+  </si>
+  <si>
+    <t>qdrn</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>m3/s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,13 +74,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,9 +109,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,89 +392,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0.01</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <f>10/3600</f>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
-      </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>0.01</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="H5" s="1"/>
+      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prep for cal 1-11 + mag fac at 100 for mr
</commit_message>
<xml_diff>
--- a/data/weights.xlsx
+++ b/data/weights.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289F3BFE-2A0C-6A47-86B4-94BC3B9A5AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEECA440-8A97-B145-AA96-DF31C5DAE2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23840" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H4" s="1"/>
     </row>

</xml_diff>

<commit_message>
weight of MR to 100
</commit_message>
<xml_diff>
--- a/data/weights.xlsx
+++ b/data/weights.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43F55D2-4355-C945-990C-1D420821A729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38CA6A8-F991-1948-9E8D-CB38426C84D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23840" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H4" s="1"/>
     </row>

</xml_diff>

<commit_message>
weight for mr to 50
</commit_message>
<xml_diff>
--- a/data/weights.xlsx
+++ b/data/weights.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38CA6A8-F991-1948-9E8D-CB38426C84D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E7BC70-2E66-FA4F-AF0D-CA13E9D6556F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23840" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H4" s="1"/>
     </row>

</xml_diff>

<commit_message>
back to w=10 for MR
</commit_message>
<xml_diff>
--- a/data/weights.xlsx
+++ b/data/weights.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E7BC70-2E66-FA4F-AF0D-CA13E9D6556F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAED5E97-F377-D848-A66A-C1227013F791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23840" windowHeight="14840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1"/>
     </row>

</xml_diff>